<commit_message>
Added stall speed constraint, changed motor sizing
</commit_message>
<xml_diff>
--- a/data/MotorSpecs.xlsx
+++ b/data/MotorSpecs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debna_3tbjgpv\Documents\Design_Build\ADOT2023-main\ADOT\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Downloads\ADOT_OO_14_12_2023_1.15_PM\ADOT 2023\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8DB130-BF91-469E-B31C-B76EC4336C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC46FD37-551A-4488-8DA8-EABA7844E98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8EC4D84A-1F87-4710-9341-B399FCA76A9C}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15435" xr2:uid="{8EC4D84A-1F87-4710-9341-B399FCA76A9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Motor" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>URL</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>https://www.modelflight.com.au/dualsky-eco-5330c-brushless-motor-225kv-3600w.html</t>
+  </si>
+  <si>
+    <t>https://hobbyking.com/en_us/turnigy-aerodrive-sk3-5045-450kv-brushless-outrunner-motor.html?___store=en_us#qa[bW9kZT03JnBhZ2U9MSZxdWVzdGlvbl9zZWFyY2hfY29udGVudD0mcT0zMTk0]</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -467,22 +473,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7E257B-E6DF-44A1-B68A-2BB00A2A6F30}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.59765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.86328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="86.86328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="86.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -499,7 +505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -516,41 +522,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>300</v>
+      </c>
+      <c r="C3" s="1">
+        <v>72</v>
+      </c>
+      <c r="D3" s="1">
+        <v>980</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>420</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="1">
         <v>104</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="1">
         <v>1350</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>300</v>
-      </c>
-      <c r="C4" s="1">
-        <v>72</v>
-      </c>
-      <c r="D4" s="1">
-        <v>980</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -567,75 +573,75 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>160</v>
+      </c>
+      <c r="D6" s="1">
+        <v>550</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1260</v>
+      </c>
+      <c r="C7" s="1">
+        <v>275</v>
+      </c>
+      <c r="D7" s="1">
+        <v>450</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B8" s="1">
         <v>1400</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C8" s="1">
         <v>355</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D8" s="1">
         <v>2100</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B9" s="1">
         <v>1400</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C9" s="1">
         <v>355</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D9" s="1">
         <v>4100</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C8" s="1">
-        <v>160</v>
-      </c>
-      <c r="D8" s="1">
-        <v>550</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2160</v>
-      </c>
-      <c r="C9" s="1">
-        <v>510</v>
-      </c>
-      <c r="D9" s="1">
-        <v>380</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -652,29 +658,58 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2160</v>
+      </c>
+      <c r="C11" s="1">
+        <v>510</v>
+      </c>
+      <c r="D11" s="1">
+        <v>380</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>3600</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <v>640</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D12" s="1">
         <v>225</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
+    <sortCondition ref="B2:B12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D7B4AA51A86DF64F8EEA3B7ACC01600E" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="37503d37778738f9b8e5b50734e360b9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5f869584-441e-42c5-8d1e-76b11125194b" xmlns:ns3="9df0515c-157b-471a-a0ef-89af1efb2dd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f630545ba42abbb2436d67874f362a0" ns2:_="" ns3:_="">
     <xsd:import namespace="5f869584-441e-42c5-8d1e-76b11125194b"/>
@@ -897,15 +932,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -918,6 +944,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A79501D-A641-46E9-8090-FFC728BDED2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB9A91A5-3E46-403A-B8FE-FB78FF3ACF94}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -936,14 +970,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A79501D-A641-46E9-8090-FFC728BDED2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E24B1721-9C5D-41CC-823C-A30077D27BE1}">
   <ds:schemaRefs>

</xml_diff>